<commit_message>
Added import students from excel functionality
</commit_message>
<xml_diff>
--- a/public/uploads/Book12.xlsx
+++ b/public/uploads/Book12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AssessmentPlatform_IKIGAI\assesment-platform\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Assessment Portal\Assessment-Portal\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA44189-BB95-463D-9B42-109750AE3D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE653CF4-FCD4-4C27-9A49-340E2A313EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
@@ -85,12 +85,6 @@
     <t>questionImage</t>
   </si>
   <si>
-    <t xml:space="preserve"> is ur name?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> are you?</t>
-  </si>
-  <si>
     <t>AimageUrl</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>Dtext</t>
+  </si>
+  <si>
+    <t>How are you dear?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> What is ur name dear?</t>
   </si>
 </sst>
 </file>
@@ -956,7 +956,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,28 +966,28 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>

</xml_diff>